<commit_message>
updated based on tickets pros(11141 1123 11104)
</commit_message>
<xml_diff>
--- a/Projects/MONDELEZDMIUS/Data/MondelezDMI_KPITemplatev2.xlsx
+++ b/Projects/MONDELEZDMIUS/Data/MondelezDMI_KPITemplatev2.xlsx
@@ -56,6 +56,9 @@
     <t xml:space="preserve">Pallet - Full - PRD</t>
   </si>
   <si>
+    <t xml:space="preserve">y</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pallet - 1/2 - PRD</t>
   </si>
   <si>
@@ -66,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve">Shippers/Hutch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">y</t>
   </si>
   <si>
     <t xml:space="preserve">Shelving Rack</t>
@@ -208,17 +208,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A44" activeCellId="0" sqref="A44:N54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.63775510204082"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,12 +306,12 @@
         <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>8</v>
@@ -322,7 +322,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>8</v>
@@ -333,7 +333,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>8</v>
@@ -344,13 +344,13 @@
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>4</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -452,6 +452,19 @@
         <v>4</v>
       </c>
     </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -471,13 +484,13 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="A44:N54 A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>